<commit_message>
update feature analysis + add different working file versions
</commit_message>
<xml_diff>
--- a/feature_analysis.xlsx
+++ b/feature_analysis.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlougheed/git/strkit_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38585A88-F1AA-7749-9E46-6D48A1A7DCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FA2CC7-06AB-2F48-9B26-5FC51AEBB6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{16302E4A-BA6C-A745-8874-1B790254E989}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$10</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>STRkit</t>
   </si>
@@ -60,6 +63,51 @@
   </si>
   <si>
     <t>Existing phased SNV incorporation</t>
+  </si>
+  <si>
+    <t>Pre-built Docker image</t>
+  </si>
+  <si>
+    <t>Explicitly forbidden</t>
+  </si>
+  <si>
+    <t>Haplotagged alignment file support</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Read-level data</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>If a dbSNV VCF is provided, STRkit will use heterozygous SNVs to call TR peaks</t>
+  </si>
+  <si>
+    <t>TRGT's license restricts it to be only used with PacBio sequencing data, and the software cannot be forked and subsequently re-distributed.</t>
+  </si>
+  <si>
+    <t>STRkit is available as a pre-built Docker image, which can be incorporated into pipelines/workflow definitions (e.g., Nextflow, WDL).</t>
+  </si>
+  <si>
+    <t>Straglr</t>
+  </si>
+  <si>
+    <t>STRkit: JSON output with read-level peak ID + sequence data</t>
+  </si>
+  <si>
+    <t>Yes (GPLv3)</t>
+  </si>
+  <si>
+    <t>Yes (GPLv2)</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>✓✓</t>
   </si>
   <si>
     <r>
@@ -67,8 +115,8 @@
         <i/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>De novo</t>
     </r>
@@ -76,52 +124,24 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Helvetica"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> proximate SNV phasing</t>
     </r>
   </si>
   <si>
-    <t>Pre-built Docker image</t>
-  </si>
-  <si>
-    <t>Explicitly forbidden</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Haplotagged alignment file support</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Read-level data</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>JSON output with read-level peak ID + sequence data</t>
-  </si>
-  <si>
-    <t>If a dbSNV VCF is provided, STRkit will use heterozygous SNVs to call TR peaks</t>
-  </si>
-  <si>
-    <t>TRGT's license restricts it to be only used with PacBio sequencing data, and the software cannot be forked and subsequently re-distributed.</t>
-  </si>
-  <si>
-    <t>STRkit is available as a pre-built Docker image, which can be incorporated into pipelines/workflow definitions (e.g., Nextflow, WDL).</t>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Theoretically works on ONT data, but forbidden by software license.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,32 +150,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Helvetica"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -174,23 +193,296 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -201,6 +493,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:F10" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B4E946EC-3854-1B45-AF37-587A7571FDA7}" name="Feature" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{57F3A7A2-1B13-FF4D-997B-1DCE61D076AD}" name="STRkit" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E4C1BEF2-9F03-874F-9A72-B0B2356CA18A}" name="LongTR" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1071D67E-3526-D441-86F9-8EBD85393162}" name="TRGT" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{F9D38ED8-BFC5-1D47-A626-D72F75DFB1AD}" name="Straglr" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5C90BC75-0EDB-F44C-9DFE-EFBE4D22EF7B}" name="Notes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,172 +827,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B62DF1-3B99-804C-9453-66E4714609C8}">
-  <dimension ref="A1:E10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="3" width="13.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="64.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" ht="17">
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="40" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="25" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="25" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="9" spans="1:6" ht="25" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="40" customHeight="1">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
+      <c r="B10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
+    <row r="11" spans="1:6">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="73" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update feature analysis table
</commit_message>
<xml_diff>
--- a/feature_analysis.xlsx
+++ b/feature_analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlougheed/git/strkit_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB92198-C578-7B4C-A9AB-12D80178F8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917EFE59-B290-7F4F-BA00-1647FEE50C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{16302E4A-BA6C-A745-8874-1B790254E989}"/>
   </bookViews>
@@ -140,6 +140,21 @@
     <t>Copy number output</t>
   </si>
   <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>Allele size confidence intervals</t>
+  </si>
+  <si>
+    <t>✓ + output</t>
+  </si>
+  <si>
+    <t>All but Straglr can used phased read data (from, e.g., WhatsHap) to call STR alleles.</t>
+  </si>
+  <si>
+    <t>STRkit and TRGT can use heterozygous SNVs to cluster STR alleles; STRkit can output them to VCF.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -176,7 +191,7 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> overlapping reads; </t>
+      <t xml:space="preserve"> overlapping reads in BAM; </t>
     </r>
     <r>
       <rPr>
@@ -214,23 +229,8 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> read-level sequences</t>
+      <t xml:space="preserve"> read-level sequence output in VCF.</t>
     </r>
-  </si>
-  <si>
-    <t>Partial</t>
-  </si>
-  <si>
-    <t>Allele size confidence intervals</t>
-  </si>
-  <si>
-    <t>✓ + output</t>
-  </si>
-  <si>
-    <t>STRkit can use heterozygous SNVs to cluster STR alleles and output them to VCF.</t>
-  </si>
-  <si>
-    <t>All but Straglr can used phased read data (from, e.g., WhatsHap) to call STR alleles.</t>
   </si>
 </sst>
 </file>
@@ -322,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -362,6 +362,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,7 +924,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -927,7 +933,7 @@
     <col min="2" max="3" width="13.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17">
@@ -937,13 +943,13 @@
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -960,13 +966,13 @@
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -976,18 +982,18 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1000,7 +1006,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -1052,14 +1058,14 @@
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="25" customHeight="1">
@@ -1117,7 +1123,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>19</v>
@@ -1126,7 +1132,7 @@
         <v>19</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="58" customHeight="1">
@@ -1165,10 +1171,10 @@
       <c r="D11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="5"/>
@@ -1198,7 +1204,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
update feature analysis xlsx
</commit_message>
<xml_diff>
--- a/feature_analysis.xlsx
+++ b/feature_analysis.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlougheed/git/strkit_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C773BBB0-646C-A146-96A6-2DC80FD7DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADCA964-B715-274A-B6D9-5F1C261B7D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{16302E4A-BA6C-A745-8874-1B790254E989}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{16302E4A-BA6C-A745-8874-1B790254E989}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>STRkit</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>TRGT's license restricts it to be only used with PacBio sequencing data, and the software cannot be forked and subsequently re-distributed.</t>
-  </si>
-  <si>
-    <t>STRkit is available as a pre-built Docker image, which can be incorporated into pipelines/workflow definitions (e.g., Nextflow, WDL).</t>
   </si>
   <si>
     <t>Straglr</t>
@@ -125,9 +122,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Theoretically works on ONT data, but forbidden by software license.</t>
-  </si>
-  <si>
     <t>STRdust</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
   </si>
   <si>
     <t>✓ + output</t>
-  </si>
-  <si>
-    <t>All but Straglr can used phased read data (from, e.g., WhatsHap) to call STR alleles.</t>
   </si>
   <si>
     <t>STRkit and TRGT can use heterozygous SNVs to cluster STR alleles; STRkit can output them to VCF.</t>
@@ -236,10 +227,43 @@
     <t xml:space="preserve">STRkit includes a tool to output loci which do not respect Mendelian inheritance in a set of trio VCFs. </t>
   </si>
   <si>
-    <t>Allele consensus sequence ouput</t>
-  </si>
-  <si>
     <t>Free and open-source software license</t>
+  </si>
+  <si>
+    <t>All but Straglr can use phased read data from, e.g., WhatsHap (Martin et al. 2016) to call STRs.</t>
+  </si>
+  <si>
+    <t>STRkit is available as a pre-built Docker image, which can be incorporated into, e.g., Nextflow pipelines.</t>
+  </si>
+  <si>
+    <t>Allele consensus sequence output</t>
+  </si>
+  <si>
+    <t>Beyond read-length genotyping</t>
+  </si>
+  <si>
+    <t>Straglr can use reads that cover only part of a repeat to support alleles, but does not have a size model which incorporates in-repeat reads like some short-read STR genotypers.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>TRGT:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> theoretically works on ONT data, but forbidden by software license.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -290,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -327,6 +351,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -375,8 +408,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,8 +628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
-  <autoFilter ref="A1:G14" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:G15" xr:uid="{460A7272-5592-CF4D-B736-14C01BA1A062}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B4E946EC-3854-1B45-AF37-587A7571FDA7}" name="Feature" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{57F3A7A2-1B13-FF4D-997B-1DCE61D076AD}" name="STRkit" dataDxfId="5"/>
@@ -930,10 +963,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="120" zoomScaleNormal="140" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -947,7 +980,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17">
       <c r="A1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -959,10 +992,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>12</v>
@@ -970,19 +1003,19 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
@@ -991,19 +1024,19 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -1015,244 +1048,267 @@
         <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="40" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
+    <row r="5" spans="1:7" ht="68">
+      <c r="A5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="25" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="40" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="25" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="34">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="34">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="34">
+      <c r="A10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="68">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="33" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="25" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="34">
-      <c r="A9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="58" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" ht="38" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="68">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="33" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="58" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="25" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="51">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>